<commit_message>
maj cours 5 ipt
</commit_message>
<xml_diff>
--- a/mpsi2_TP_2020_2021.xlsx
+++ b/mpsi2_TP_2020_2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="1120" windowWidth="19400" windowHeight="14220" activeTab="1"/>
+    <workbookView xWindow="6200" yWindow="1000" windowWidth="19400" windowHeight="14220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="S2" sheetId="2" r:id="rId1"/>
@@ -2432,7 +2432,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2483,7 +2483,9 @@
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2501,7 +2503,9 @@
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2519,7 +2523,9 @@
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2537,7 +2543,9 @@
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2555,7 +2563,9 @@
       <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2573,7 +2583,9 @@
       <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2591,7 +2603,9 @@
       <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2609,7 +2623,9 @@
       <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2625,7 +2641,9 @@
         <v>47</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2640,8 +2658,12 @@
       <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2659,7 +2681,9 @@
       <c r="C12" s="2">
         <v>1</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -2674,8 +2698,12 @@
       <c r="B13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -2691,7 +2719,9 @@
         <v>47</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2707,7 +2737,9 @@
         <v>47</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -2723,7 +2755,9 @@
         <v>47</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -2862,7 +2896,9 @@
       <c r="B24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -2878,7 +2914,9 @@
       <c r="B25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2894,7 +2932,9 @@
       <c r="B26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2910,7 +2950,9 @@
       <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -2926,7 +2968,9 @@
       <c r="B28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -3056,7 +3100,9 @@
       <c r="B36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -3072,7 +3118,9 @@
       <c r="B37" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -3088,7 +3136,9 @@
       <c r="B38" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>

</xml_diff>

<commit_message>
maj info cours 2-2 et TP9
</commit_message>
<xml_diff>
--- a/mpsi2_TP_2020_2021.xlsx
+++ b/mpsi2_TP_2020_2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="12840" yWindow="460" windowWidth="12760" windowHeight="14560" activeTab="1"/>
+    <workbookView xWindow="2860" yWindow="480" windowWidth="16860" windowHeight="14560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="S2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
   <si>
     <t>Nom et prénom</t>
   </si>
@@ -192,9 +192,6 @@
     <t>TP05</t>
   </si>
   <si>
-    <t>TP06</t>
-  </si>
-  <si>
     <t>TP08</t>
   </si>
   <si>
@@ -361,6 +358,12 @@
   </si>
   <si>
     <t xml:space="preserve">ZAZA AUTHIER </t>
+  </si>
+  <si>
+    <t>NGOM</t>
+  </si>
+  <si>
+    <t>TP06-7</t>
   </si>
 </sst>
 </file>
@@ -785,31 +788,31 @@
         <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -972,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
@@ -2423,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2458,18 +2461,18 @@
         <v>53</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>47</v>
@@ -2486,14 +2489,16 @@
       <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>47</v>
@@ -2510,14 +2515,18 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>47</v>
@@ -2534,14 +2543,16 @@
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>47</v>
@@ -2558,14 +2569,18 @@
       <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>47</v>
@@ -2580,14 +2595,18 @@
       <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>47</v>
@@ -2604,14 +2623,18 @@
       <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>47</v>
@@ -2628,14 +2651,18 @@
       <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>47</v>
@@ -2652,14 +2679,18 @@
       <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>47</v>
@@ -2674,14 +2705,18 @@
       <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>47</v>
@@ -2698,14 +2733,16 @@
       <c r="F11" s="2">
         <v>1</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>47</v>
@@ -2722,43 +2759,43 @@
       <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
       <c r="D14" s="3">
         <v>1</v>
       </c>
@@ -2768,14 +2805,18 @@
       <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>47</v>
@@ -2790,74 +2831,86 @@
       <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1</v>
-      </c>
-      <c r="G17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>72</v>
+      <c r="A18" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>48</v>
@@ -2871,17 +2924,17 @@
       <c r="E19" s="2">
         <v>1</v>
       </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>82</v>
+      <c r="A20" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>48</v>
@@ -2889,23 +2942,27 @@
       <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>48</v>
@@ -2919,15 +2976,21 @@
       <c r="E21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>87</v>
+      <c r="A22" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>48</v>
@@ -2935,23 +2998,23 @@
       <c r="C22" s="2">
         <v>1</v>
       </c>
-      <c r="D22" s="2">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>48</v>
@@ -2968,14 +3031,18 @@
       <c r="F23" s="2">
         <v>1</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>48</v>
@@ -2992,14 +3059,18 @@
       <c r="F24" s="2">
         <v>1</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>91</v>
+      <c r="A25" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>48</v>
@@ -3007,23 +3078,27 @@
       <c r="C25" s="2">
         <v>1</v>
       </c>
-      <c r="D25" s="3">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>48</v>
@@ -3031,146 +3106,176 @@
       <c r="C26" s="2">
         <v>1</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
       <c r="E26" s="3">
         <v>1</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>96</v>
+      <c r="A27" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>98</v>
+      <c r="A28" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3">
-        <v>1</v>
-      </c>
-      <c r="F28" s="3">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>102</v>
+      <c r="A29" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3">
-        <v>1</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+      <c r="A31" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>75</v>
+      <c r="A32" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="2">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -3181,25 +3286,25 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="2">
-        <v>1</v>
-      </c>
+      <c r="C34" s="2"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>92</v>
+      <c r="A35" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>49</v>
@@ -3207,17 +3312,17 @@
       <c r="C35" s="2">
         <v>1</v>
       </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>49</v>
@@ -3234,40 +3339,42 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>97</v>
+      <c r="A37" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>99</v>
+      <c r="A38" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>49</v>
@@ -3277,34 +3384,36 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+      <c r="H39" s="2">
+        <v>1</v>
+      </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>101</v>
+      <c r="A40" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="3"/>
+      <c r="C41" s="2"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -3314,24 +3423,26 @@
       <c r="J41" s="3"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3">
+        <v>1</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>49</v>
@@ -3346,36 +3457,52 @@
       <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B44" s="3" t="s">
+      <c r="A44" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B45" s="8" t="s">
+      <c r="A45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:J47">

</xml_diff>